<commit_message>
Corregido casos de prueba
</commit_message>
<xml_diff>
--- a/3SCRUM/Excel-Burndown-Chart-Template.xlsx
+++ b/3SCRUM/Excel-Burndown-Chart-Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emili\Desktop\ProyectoMetodologia\proyectometodologia7342\proyectometodologia7342\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emili\Desktop\ProyectoMetodologia\proyectometodologia7342\proyectometodologia7342\3SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660C7419-25F4-49A3-B3D2-97E1C9C2F7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6555AD-AE7C-4942-A556-1755FAF286F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="4" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="171">
   <si>
     <t>Start Date</t>
   </si>
@@ -263,9 +263,6 @@
     <t>Terminado</t>
   </si>
   <si>
-    <t>Agregar un proveedor</t>
-  </si>
-  <si>
     <t>Agregar productos</t>
   </si>
   <si>
@@ -443,12 +440,6 @@
     <t>Registrar datos del cliente</t>
   </si>
   <si>
-    <t>Modificar datos del cliente</t>
-  </si>
-  <si>
-    <t>actualizar datos del cliente</t>
-  </si>
-  <si>
     <t>VP13</t>
   </si>
   <si>
@@ -596,12 +587,6 @@
     <t>agregar datos generales de empleados</t>
   </si>
   <si>
-    <t>Modificar datos de empleados</t>
-  </si>
-  <si>
-    <t>actualizar datos de empleados</t>
-  </si>
-  <si>
     <t>Crear tablas y campos de base de datos (clientes etc)</t>
   </si>
   <si>
@@ -639,6 +624,18 @@
   </si>
   <si>
     <t>7</t>
+  </si>
+  <si>
+    <t>Modificar datos del cliente y empleados</t>
+  </si>
+  <si>
+    <t>actualizar datos del cliente y empleados</t>
+  </si>
+  <si>
+    <t>Agregar categorias</t>
+  </si>
+  <si>
+    <t>Dividir los productos en categorias</t>
   </si>
 </sst>
 </file>
@@ -1295,17 +1292,17 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5843,7 +5840,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5855,7 +5852,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>35</v>
@@ -5881,340 +5878,340 @@
     </row>
     <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="D2" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>104</v>
-      </c>
       <c r="F2" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G3" s="26" t="s">
         <v>44</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>106</v>
+        <v>167</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G5" s="26" t="s">
         <v>44</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G6" s="26" t="s">
         <v>44</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>44</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G8" s="26" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D9" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="23" t="s">
-        <v>53</v>
-      </c>
       <c r="F9" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G10" s="26" t="s">
         <v>44</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G11" s="26" t="s">
         <v>44</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>103</v>
-      </c>
       <c r="D13" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F13" s="61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G13" s="26" t="s">
         <v>44</v>
       </c>
       <c r="H13" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="30" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C14" s="62" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D14" s="62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F14" s="61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G14" s="63" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -6226,8 +6223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6248,16 +6245,16 @@
         <v>36</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>10</v>
@@ -6275,10 +6272,10 @@
         <v>43</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="20" t="s">
@@ -6292,32 +6289,32 @@
       <c r="A3" s="19"/>
       <c r="B3" s="38"/>
       <c r="C3" s="39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="40"/>
       <c r="E3" s="40"/>
       <c r="F3" s="40"/>
       <c r="G3" s="39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H3" s="40"/>
       <c r="I3" s="41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="85" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+        <v>69</v>
+      </c>
+      <c r="C4" s="81" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
       <c r="G4" s="43" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H4" s="43"/>
       <c r="I4" s="44">
@@ -6327,16 +6324,16 @@
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
       <c r="B5" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" s="81" t="s">
-        <v>159</v>
-      </c>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
+        <v>88</v>
+      </c>
+      <c r="C5" s="83" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
       <c r="G5" s="46" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H5" s="46"/>
       <c r="I5" s="47">
@@ -6346,13 +6343,13 @@
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
       <c r="G6" s="18"/>
       <c r="H6" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I6" s="56">
         <f>SUM(I4:I5)</f>
@@ -6371,16 +6368,16 @@
         <v>36</v>
       </c>
       <c r="E7" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>10</v>
@@ -6395,13 +6392,13 @@
         <v>42</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>46</v>
+        <v>63</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>152</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20" t="s">
@@ -6415,32 +6412,32 @@
       <c r="A9" s="19"/>
       <c r="B9" s="18"/>
       <c r="C9" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="79" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
+        <v>70</v>
+      </c>
+      <c r="C10" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
       <c r="G10" s="40" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H10" s="40"/>
       <c r="I10" s="48">
@@ -6450,16 +6447,16 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
       <c r="B11" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="85" t="s">
-        <v>122</v>
-      </c>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
+        <v>71</v>
+      </c>
+      <c r="C11" s="81" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
       <c r="G11" s="43" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H11" s="43"/>
       <c r="I11" s="44">
@@ -6469,16 +6466,16 @@
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
       <c r="B12" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="81" t="s">
-        <v>160</v>
-      </c>
-      <c r="D12" s="82"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="82"/>
+        <v>87</v>
+      </c>
+      <c r="C12" s="83" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84"/>
       <c r="G12" s="46" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H12" s="46"/>
       <c r="I12" s="49">
@@ -6488,13 +6485,13 @@
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="18"/>
-      <c r="C13" s="78"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="79"/>
       <c r="G13" s="18"/>
       <c r="H13" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I13" s="56">
         <f>SUM(I10:I12)</f>
@@ -6513,16 +6510,16 @@
         <v>36</v>
       </c>
       <c r="E14" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>10</v>
@@ -6540,10 +6537,10 @@
         <v>43</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>106</v>
+        <v>167</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="20" t="s">
@@ -6557,32 +6554,32 @@
       <c r="A16" s="19"/>
       <c r="B16" s="18"/>
       <c r="C16" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="79" t="s">
-        <v>161</v>
-      </c>
-      <c r="D17" s="80"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80"/>
+        <v>73</v>
+      </c>
+      <c r="C17" s="85" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
       <c r="G17" s="40" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H17" s="40"/>
       <c r="I17" s="48">
@@ -6592,16 +6589,16 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="85" t="s">
-        <v>162</v>
-      </c>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
+        <v>74</v>
+      </c>
+      <c r="C18" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="82"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="82"/>
       <c r="G18" s="43" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H18" s="43"/>
       <c r="I18" s="44">
@@ -6611,16 +6608,16 @@
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
       <c r="B19" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="81" t="s">
-        <v>163</v>
-      </c>
-      <c r="D19" s="82"/>
-      <c r="E19" s="82"/>
-      <c r="F19" s="82"/>
+        <v>72</v>
+      </c>
+      <c r="C19" s="83" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="84"/>
       <c r="G19" s="46" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H19" s="46"/>
       <c r="I19" s="47">
@@ -6636,7 +6633,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="H20" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I20" s="56">
         <f>SUM(I17:I19)</f>
@@ -6655,16 +6652,16 @@
         <v>36</v>
       </c>
       <c r="E21" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I21" s="17" t="s">
         <v>10</v>
@@ -6682,10 +6679,10 @@
         <v>43</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="24" t="s">
-        <v>150</v>
+        <v>169</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>170</v>
       </c>
       <c r="G22" s="21"/>
       <c r="H22" s="20" t="s">
@@ -6699,32 +6696,32 @@
       <c r="A23" s="19"/>
       <c r="B23" s="18"/>
       <c r="C23" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="79" t="s">
-        <v>126</v>
-      </c>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="80"/>
+        <v>75</v>
+      </c>
+      <c r="C24" s="85" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
       <c r="G24" s="40" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H24" s="40"/>
       <c r="I24" s="48">
@@ -6734,16 +6731,16 @@
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" s="84" t="s">
-        <v>141</v>
-      </c>
-      <c r="D25" s="84"/>
-      <c r="E25" s="84"/>
-      <c r="F25" s="84"/>
+        <v>76</v>
+      </c>
+      <c r="C25" s="80" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
       <c r="G25" s="46" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H25" s="46"/>
       <c r="I25" s="47">
@@ -6753,13 +6750,13 @@
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="18"/>
-      <c r="C26" s="83"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="78"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="79"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="79"/>
       <c r="G26" s="18"/>
       <c r="H26" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I26" s="56">
         <f>SUM(I24:I25)</f>
@@ -6778,16 +6775,16 @@
         <v>36</v>
       </c>
       <c r="E27" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I27" s="17" t="s">
         <v>10</v>
@@ -6805,10 +6802,10 @@
         <v>43</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="F28" s="23" t="s">
-        <v>158</v>
+        <v>46</v>
+      </c>
+      <c r="F28" s="24" t="s">
+        <v>147</v>
       </c>
       <c r="G28" s="21"/>
       <c r="H28" s="20" t="s">
@@ -6833,32 +6830,32 @@
       <c r="A30" s="19"/>
       <c r="B30" s="18"/>
       <c r="C30" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H30" s="18"/>
       <c r="I30" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="B31" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="79" t="s">
-        <v>164</v>
-      </c>
-      <c r="D31" s="80"/>
-      <c r="E31" s="80"/>
-      <c r="F31" s="80"/>
+        <v>77</v>
+      </c>
+      <c r="C31" s="85" t="s">
+        <v>159</v>
+      </c>
+      <c r="D31" s="86"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="86"/>
       <c r="G31" s="40" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H31" s="40"/>
       <c r="I31" s="48">
@@ -6868,16 +6865,16 @@
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
       <c r="B32" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="81" t="s">
-        <v>165</v>
-      </c>
-      <c r="D32" s="82"/>
-      <c r="E32" s="82"/>
-      <c r="F32" s="82"/>
+        <v>78</v>
+      </c>
+      <c r="C32" s="83" t="s">
+        <v>160</v>
+      </c>
+      <c r="D32" s="84"/>
+      <c r="E32" s="84"/>
+      <c r="F32" s="84"/>
       <c r="G32" s="46" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H32" s="46"/>
       <c r="I32" s="47">
@@ -6893,7 +6890,7 @@
       <c r="F33" s="19"/>
       <c r="G33" s="18"/>
       <c r="H33" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I33" s="56">
         <f>SUM(I31:I32)</f>
@@ -6912,16 +6909,16 @@
         <v>36</v>
       </c>
       <c r="E34" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I34" s="17" t="s">
         <v>10</v>
@@ -6939,10 +6936,10 @@
         <v>43</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G35" s="21"/>
       <c r="H35" s="20" t="s">
@@ -6956,32 +6953,32 @@
       <c r="A36" s="19"/>
       <c r="B36" s="18"/>
       <c r="C36" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H36" s="18"/>
       <c r="I36" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
       <c r="B37" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="C37" s="79" t="s">
-        <v>166</v>
-      </c>
-      <c r="D37" s="80"/>
-      <c r="E37" s="80"/>
-      <c r="F37" s="80"/>
+        <v>79</v>
+      </c>
+      <c r="C37" s="85" t="s">
+        <v>161</v>
+      </c>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="86"/>
       <c r="G37" s="40" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H37" s="40"/>
       <c r="I37" s="48">
@@ -6991,16 +6988,16 @@
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19"/>
       <c r="B38" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="81" t="s">
-        <v>167</v>
-      </c>
-      <c r="D38" s="82"/>
-      <c r="E38" s="82"/>
-      <c r="F38" s="82"/>
+        <v>80</v>
+      </c>
+      <c r="C38" s="83" t="s">
+        <v>162</v>
+      </c>
+      <c r="D38" s="84"/>
+      <c r="E38" s="84"/>
+      <c r="F38" s="84"/>
       <c r="G38" s="46" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H38" s="46"/>
       <c r="I38" s="47">
@@ -7010,13 +7007,13 @@
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19"/>
       <c r="B39" s="18"/>
-      <c r="C39" s="78"/>
-      <c r="D39" s="78"/>
-      <c r="E39" s="78"/>
-      <c r="F39" s="78"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="79"/>
+      <c r="E39" s="79"/>
+      <c r="F39" s="79"/>
       <c r="G39" s="18"/>
       <c r="H39" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I39" s="56">
         <f>SUM(I37:I38)</f>
@@ -7035,16 +7032,16 @@
         <v>36</v>
       </c>
       <c r="E40" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F40" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="G40" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I40" s="17" t="s">
         <v>10</v>
@@ -7062,10 +7059,10 @@
         <v>43</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F41" s="23" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G41" s="21"/>
       <c r="H41" s="20" t="s">
@@ -7079,32 +7076,32 @@
       <c r="A42" s="19"/>
       <c r="B42" s="71"/>
       <c r="C42" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D42" s="71"/>
       <c r="E42" s="71"/>
       <c r="F42" s="71"/>
       <c r="G42" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H42" s="71"/>
       <c r="I42" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
       <c r="B43" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="C43" s="79" t="s">
-        <v>168</v>
-      </c>
-      <c r="D43" s="80"/>
-      <c r="E43" s="80"/>
-      <c r="F43" s="80"/>
+        <v>81</v>
+      </c>
+      <c r="C43" s="85" t="s">
+        <v>163</v>
+      </c>
+      <c r="D43" s="86"/>
+      <c r="E43" s="86"/>
+      <c r="F43" s="86"/>
       <c r="G43" s="69" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H43" s="69"/>
       <c r="I43" s="48">
@@ -7114,16 +7111,16 @@
     <row r="44" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="19"/>
       <c r="B44" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="C44" s="81" t="s">
-        <v>169</v>
-      </c>
-      <c r="D44" s="82"/>
-      <c r="E44" s="82"/>
-      <c r="F44" s="82"/>
+        <v>82</v>
+      </c>
+      <c r="C44" s="83" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" s="84"/>
+      <c r="E44" s="84"/>
+      <c r="F44" s="84"/>
       <c r="G44" s="70" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H44" s="70"/>
       <c r="I44" s="47">
@@ -7133,13 +7130,13 @@
     <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19"/>
       <c r="B45" s="71"/>
-      <c r="C45" s="78"/>
-      <c r="D45" s="78"/>
-      <c r="E45" s="78"/>
-      <c r="F45" s="78"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="79"/>
+      <c r="E45" s="79"/>
+      <c r="F45" s="79"/>
       <c r="G45" s="71"/>
       <c r="H45" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I45" s="56">
         <f>SUM(I43:I44)</f>
@@ -7161,7 +7158,7 @@
     <row r="50" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A50" s="19"/>
       <c r="H50" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I50" s="51">
         <f>SUM(I6,I13,I20,I26,I33,I39,I45)</f>
@@ -7216,6 +7213,14 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C39:F39"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="C4:F4"/>
@@ -7229,14 +7234,6 @@
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C39:F39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7264,16 +7261,16 @@
         <v>36</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>10</v>
@@ -7287,13 +7284,13 @@
         <v>42</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>48</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>49</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="20" t="s">
@@ -7306,31 +7303,31 @@
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="18"/>
       <c r="C3" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="79" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
+        <v>81</v>
+      </c>
+      <c r="C4" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="40" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H4" s="40"/>
       <c r="I4" s="48">
@@ -7339,16 +7336,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="85" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
+        <v>82</v>
+      </c>
+      <c r="C5" s="81" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
       <c r="G5" s="43" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H5" s="43"/>
       <c r="I5" s="44">
@@ -7357,16 +7354,16 @@
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="81" t="s">
-        <v>130</v>
-      </c>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
+        <v>83</v>
+      </c>
+      <c r="C6" s="83" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
       <c r="G6" s="46" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H6" s="46"/>
       <c r="I6" s="47">
@@ -7381,7 +7378,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I7" s="56">
         <f>SUM(I4:I6)</f>
@@ -7399,16 +7396,16 @@
         <v>36</v>
       </c>
       <c r="E8" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I8" s="17" t="s">
         <v>10</v>
@@ -7425,10 +7422,10 @@
         <v>43</v>
       </c>
       <c r="E9" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="20" t="s">
         <v>50</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>51</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="20" t="s">
@@ -7441,31 +7438,31 @@
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="18"/>
       <c r="C10" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
       <c r="G10" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="79" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
+        <v>84</v>
+      </c>
+      <c r="C11" s="85" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
       <c r="G11" s="40" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H11" s="40"/>
       <c r="I11" s="48">
@@ -7474,16 +7471,16 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="85" t="s">
-        <v>132</v>
-      </c>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
+        <v>85</v>
+      </c>
+      <c r="C12" s="81" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
       <c r="G12" s="43" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H12" s="43"/>
       <c r="I12" s="44">
@@ -7492,16 +7489,16 @@
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="81" t="s">
-        <v>133</v>
-      </c>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
+        <v>86</v>
+      </c>
+      <c r="C13" s="83" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="84"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="84"/>
       <c r="G13" s="46" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H13" s="46"/>
       <c r="I13" s="47">
@@ -7510,7 +7507,7 @@
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H14" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I14" s="56">
         <f>SUM(I11:I13)</f>
@@ -7538,16 +7535,16 @@
         <v>36</v>
       </c>
       <c r="E16" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>10</v>
@@ -7564,10 +7561,10 @@
         <v>43</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G17" s="21"/>
       <c r="H17" s="20" t="s">
@@ -7580,31 +7577,31 @@
     <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="60"/>
       <c r="C18" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="60"/>
       <c r="E18" s="60"/>
       <c r="F18" s="60"/>
       <c r="G18" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H18" s="60"/>
       <c r="I18" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="C19" s="79" t="s">
-        <v>134</v>
-      </c>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="79"/>
+        <v>143</v>
+      </c>
+      <c r="C19" s="85" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
       <c r="G19" s="57" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H19" s="57"/>
       <c r="I19" s="48">
@@ -7613,16 +7610,16 @@
     </row>
     <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="45" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C20" s="59" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D20" s="59"/>
       <c r="E20" s="59"/>
       <c r="F20" s="59"/>
       <c r="G20" s="59" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H20" s="59"/>
       <c r="I20" s="47">
@@ -7631,13 +7628,13 @@
     </row>
     <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="60"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="79"/>
-      <c r="F21" s="79"/>
+      <c r="C21" s="85"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="85"/>
+      <c r="F21" s="85"/>
       <c r="G21" s="60"/>
       <c r="H21" s="54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I21" s="55">
         <f>SUM(I19:I20)</f>
@@ -7665,16 +7662,16 @@
         <v>36</v>
       </c>
       <c r="E23" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I23" s="17" t="s">
         <v>10</v>
@@ -7691,10 +7688,10 @@
         <v>43</v>
       </c>
       <c r="E24" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" s="20" t="s">
         <v>55</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>56</v>
       </c>
       <c r="G24" s="21"/>
       <c r="H24" s="20" t="s">
@@ -7707,31 +7704,31 @@
     <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="60"/>
       <c r="C25" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25" s="60"/>
       <c r="E25" s="60"/>
       <c r="F25" s="60"/>
       <c r="G25" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H25" s="60"/>
       <c r="I25" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="C26" s="79" t="s">
-        <v>136</v>
-      </c>
-      <c r="D26" s="79"/>
-      <c r="E26" s="79"/>
-      <c r="F26" s="79"/>
+        <v>140</v>
+      </c>
+      <c r="C26" s="85" t="s">
+        <v>133</v>
+      </c>
+      <c r="D26" s="85"/>
+      <c r="E26" s="85"/>
+      <c r="F26" s="85"/>
       <c r="G26" s="57" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H26" s="57"/>
       <c r="I26" s="48">
@@ -7740,16 +7737,16 @@
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C27" s="79" t="s">
-        <v>138</v>
-      </c>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="79"/>
+        <v>141</v>
+      </c>
+      <c r="C27" s="85" t="s">
+        <v>135</v>
+      </c>
+      <c r="D27" s="85"/>
+      <c r="E27" s="85"/>
+      <c r="F27" s="85"/>
       <c r="G27" s="58" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H27" s="58"/>
       <c r="I27" s="44">
@@ -7758,16 +7755,16 @@
     </row>
     <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="45" t="s">
-        <v>148</v>
-      </c>
-      <c r="C28" s="81" t="s">
-        <v>137</v>
-      </c>
-      <c r="D28" s="81"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81"/>
+        <v>145</v>
+      </c>
+      <c r="C28" s="83" t="s">
+        <v>134</v>
+      </c>
+      <c r="D28" s="83"/>
+      <c r="E28" s="83"/>
+      <c r="F28" s="83"/>
       <c r="G28" s="59" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H28" s="59"/>
       <c r="I28" s="47">
@@ -7776,16 +7773,16 @@
     </row>
     <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="45" t="s">
-        <v>149</v>
-      </c>
-      <c r="C29" s="81" t="s">
-        <v>139</v>
-      </c>
-      <c r="D29" s="81"/>
-      <c r="E29" s="81"/>
-      <c r="F29" s="81"/>
+        <v>146</v>
+      </c>
+      <c r="C29" s="83" t="s">
+        <v>136</v>
+      </c>
+      <c r="D29" s="83"/>
+      <c r="E29" s="83"/>
+      <c r="F29" s="83"/>
       <c r="G29" s="59" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H29" s="59"/>
       <c r="I29" s="47">
@@ -7794,7 +7791,7 @@
     </row>
     <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H30" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I30" s="53">
         <f>SUM(I26:I29)</f>
@@ -7803,7 +7800,7 @@
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H31" s="50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I31" s="50">
         <f>I14+I7+I21+I30</f>
@@ -7812,18 +7809,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C26:F26"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C26:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8022,16 +8019,16 @@
         <v>5</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F3" s="11">
         <v>2</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -8046,16 +8043,16 @@
         <v>6</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F4" s="11">
         <v>4</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -8070,16 +8067,16 @@
         <v>5</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F5" s="11">
         <v>2</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -8094,16 +8091,16 @@
         <v>6</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F6" s="11">
         <v>3</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -8118,16 +8115,16 @@
         <v>5</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F7" s="11">
         <v>3</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -8142,16 +8139,16 @@
         <v>5</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F8" s="11">
         <v>3</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -8166,16 +8163,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F9" s="11">
         <v>2</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -8190,16 +8187,16 @@
         <v>7</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F10" s="11">
         <v>6</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -8214,16 +8211,16 @@
         <v>5</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F11" s="11">
         <v>2</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -8238,16 +8235,16 @@
         <v>8</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F12" s="11">
         <v>8</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -8262,16 +8259,16 @@
         <v>6</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E13" s="67" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F13" s="64">
         <v>4</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -8286,16 +8283,16 @@
         <v>7</v>
       </c>
       <c r="D14" s="64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E14" s="67" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F14" s="64">
         <v>6</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -8310,17 +8307,17 @@
         <v>7</v>
       </c>
       <c r="D15" s="64" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E15" s="67" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F15" s="64">
         <f>SprintBacklog[[#This Row],[Estimated Hours]]</f>
         <v>7</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -8335,65 +8332,65 @@
         <v>7</v>
       </c>
       <c r="D16" s="64" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E16" s="67" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F16" s="64">
         <f>SprintBacklog[[#This Row],[Estimated Hours]]</f>
         <v>7</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="64" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B17" s="65">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="C17" s="66" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D17" s="64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E17" s="67" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F17" s="64" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="73" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B18" s="74">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="C18" s="75" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D18" s="73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E18" s="76" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F18" s="73">
         <v>14</v>
       </c>
       <c r="G18" s="77" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -8618,16 +8615,16 @@
         <v>9</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F3" s="11">
         <v>7</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -8642,16 +8639,16 @@
         <v>7</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F4" s="11">
         <v>3</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -8666,16 +8663,16 @@
         <v>8</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F5" s="11">
         <v>4</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -8690,16 +8687,16 @@
         <v>8</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F6" s="11">
         <v>7</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -8714,16 +8711,16 @@
         <v>9</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F7" s="11">
         <v>2</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -8738,16 +8735,16 @@
         <v>8</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F8" s="11">
         <v>6</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -8762,16 +8759,16 @@
         <v>7</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F9" s="11">
         <v>5</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -8786,16 +8783,16 @@
         <v>9</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F10" s="11">
         <v>3</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -8810,16 +8807,16 @@
         <v>8</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F11" s="11">
         <v>8</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -8834,16 +8831,16 @@
         <v>7</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F12" s="11">
         <v>3</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -8858,16 +8855,16 @@
         <v>6</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E13" s="67" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F13" s="64">
         <v>1</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -8882,16 +8879,16 @@
         <v>10</v>
       </c>
       <c r="D14" s="64" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E14" s="67" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F14" s="64">
         <v>10</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -8928,7 +8925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cambiado texto de gerente por gerente/cajero
</commit_message>
<xml_diff>
--- a/3SCRUM/Excel-Burndown-Chart-Template.xlsx
+++ b/3SCRUM/Excel-Burndown-Chart-Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emili\Desktop\ProyectoMetodologia\proyectometodologia7342\proyectometodologia7342\3SCRUM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Desktop\New folder (3)\New folder\New folder (2)\New folder\New folder (2)\ProyectoMetodologia\proyectometodologia7342\3SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6555AD-AE7C-4942-A556-1755FAF286F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692CF211-6F63-4151-9431-00D7AA4E544F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="4" r:id="rId1"/>
@@ -46,7 +46,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -123,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="172">
   <si>
     <t>Start Date</t>
   </si>
@@ -636,6 +638,9 @@
   </si>
   <si>
     <t>Dividir los productos en categorias</t>
+  </si>
+  <si>
+    <t>Gerente/Cajero</t>
   </si>
 </sst>
 </file>
@@ -1292,21 +1297,21 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="58">
     <dxf>
@@ -1872,7 +1877,7 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -2488,7 +2493,7 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -2568,7 +2573,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2635,7 +2640,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-EC"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3286,7 +3291,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-EC"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="239344120"/>
@@ -3345,7 +3350,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-EC"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="239343728"/>
@@ -3387,7 +3392,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-EC"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3417,7 +3422,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-EC"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3431,7 +3436,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3498,7 +3503,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-EC"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4165,7 +4170,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-EC"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="239345296"/>
@@ -4224,7 +4229,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-EC"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="239344904"/>
@@ -4266,7 +4271,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-EC"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4296,7 +4301,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-EC"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5839,11 +5844,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="31.7109375" customWidth="1"/>
     <col min="5" max="5" width="63.85546875" customWidth="1"/>
@@ -6223,14 +6228,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6269,7 +6274,7 @@
         <v>42</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>43</v>
+        <v>171</v>
       </c>
       <c r="E2" s="32" t="s">
         <v>104</v>
@@ -6307,12 +6312,12 @@
       <c r="B4" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="85" t="s">
         <v>115</v>
       </c>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="43" t="s">
         <v>121</v>
       </c>
@@ -6326,12 +6331,12 @@
       <c r="B5" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="81" t="s">
         <v>154</v>
       </c>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
       <c r="G5" s="46" t="s">
         <v>116</v>
       </c>
@@ -6343,10 +6348,10 @@
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
       <c r="G6" s="18"/>
       <c r="H6" s="52" t="s">
         <v>68</v>
@@ -6430,12 +6435,12 @@
       <c r="B10" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="85" t="s">
+      <c r="C10" s="79" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
       <c r="G10" s="40" t="s">
         <v>118</v>
       </c>
@@ -6449,12 +6454,12 @@
       <c r="B11" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="81" t="s">
+      <c r="C11" s="85" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="82"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
       <c r="G11" s="43" t="s">
         <v>116</v>
       </c>
@@ -6468,12 +6473,12 @@
       <c r="B12" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="83" t="s">
+      <c r="C12" s="81" t="s">
         <v>155</v>
       </c>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
       <c r="G12" s="46" t="s">
         <v>120</v>
       </c>
@@ -6485,10 +6490,10 @@
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="18"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="79"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="79"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
       <c r="G13" s="18"/>
       <c r="H13" s="52" t="s">
         <v>68</v>
@@ -6572,12 +6577,12 @@
       <c r="B17" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="85" t="s">
+      <c r="C17" s="79" t="s">
         <v>156</v>
       </c>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80"/>
       <c r="G17" s="40" t="s">
         <v>122</v>
       </c>
@@ -6591,12 +6596,12 @@
       <c r="B18" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="81" t="s">
+      <c r="C18" s="85" t="s">
         <v>157</v>
       </c>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="82"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
       <c r="G18" s="43" t="s">
         <v>118</v>
       </c>
@@ -6610,12 +6615,12 @@
       <c r="B19" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="83" t="s">
+      <c r="C19" s="81" t="s">
         <v>158</v>
       </c>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="84"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
       <c r="G19" s="46" t="s">
         <v>116</v>
       </c>
@@ -6714,12 +6719,12 @@
       <c r="B24" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="85" t="s">
+      <c r="C24" s="79" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
       <c r="G24" s="40" t="s">
         <v>120</v>
       </c>
@@ -6733,12 +6738,12 @@
       <c r="B25" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="80" t="s">
+      <c r="C25" s="84" t="s">
         <v>138</v>
       </c>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="84"/>
       <c r="G25" s="46" t="s">
         <v>121</v>
       </c>
@@ -6750,10 +6755,10 @@
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="18"/>
-      <c r="C26" s="78"/>
-      <c r="D26" s="79"/>
-      <c r="E26" s="79"/>
-      <c r="F26" s="79"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
       <c r="G26" s="18"/>
       <c r="H26" s="52" t="s">
         <v>68</v>
@@ -6848,12 +6853,12 @@
       <c r="B31" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="85" t="s">
+      <c r="C31" s="79" t="s">
         <v>159</v>
       </c>
-      <c r="D31" s="86"/>
-      <c r="E31" s="86"/>
-      <c r="F31" s="86"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="80"/>
       <c r="G31" s="40" t="s">
         <v>116</v>
       </c>
@@ -6867,12 +6872,12 @@
       <c r="B32" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="83" t="s">
+      <c r="C32" s="81" t="s">
         <v>160</v>
       </c>
-      <c r="D32" s="84"/>
-      <c r="E32" s="84"/>
-      <c r="F32" s="84"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="82"/>
       <c r="G32" s="46" t="s">
         <v>120</v>
       </c>
@@ -6971,12 +6976,12 @@
       <c r="B37" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="85" t="s">
+      <c r="C37" s="79" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="86"/>
-      <c r="E37" s="86"/>
-      <c r="F37" s="86"/>
+      <c r="D37" s="80"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="80"/>
       <c r="G37" s="40" t="s">
         <v>118</v>
       </c>
@@ -6990,12 +6995,12 @@
       <c r="B38" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="83" t="s">
+      <c r="C38" s="81" t="s">
         <v>162</v>
       </c>
-      <c r="D38" s="84"/>
-      <c r="E38" s="84"/>
-      <c r="F38" s="84"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="82"/>
       <c r="G38" s="46" t="s">
         <v>122</v>
       </c>
@@ -7007,10 +7012,10 @@
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19"/>
       <c r="B39" s="18"/>
-      <c r="C39" s="79"/>
-      <c r="D39" s="79"/>
-      <c r="E39" s="79"/>
-      <c r="F39" s="79"/>
+      <c r="C39" s="78"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="78"/>
       <c r="G39" s="18"/>
       <c r="H39" s="52" t="s">
         <v>68</v>
@@ -7094,12 +7099,12 @@
       <c r="B43" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="C43" s="85" t="s">
+      <c r="C43" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="D43" s="86"/>
-      <c r="E43" s="86"/>
-      <c r="F43" s="86"/>
+      <c r="D43" s="80"/>
+      <c r="E43" s="80"/>
+      <c r="F43" s="80"/>
       <c r="G43" s="69" t="s">
         <v>118</v>
       </c>
@@ -7113,12 +7118,12 @@
       <c r="B44" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="83" t="s">
+      <c r="C44" s="81" t="s">
         <v>164</v>
       </c>
-      <c r="D44" s="84"/>
-      <c r="E44" s="84"/>
-      <c r="F44" s="84"/>
+      <c r="D44" s="82"/>
+      <c r="E44" s="82"/>
+      <c r="F44" s="82"/>
       <c r="G44" s="70" t="s">
         <v>116</v>
       </c>
@@ -7130,10 +7135,10 @@
     <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19"/>
       <c r="B45" s="71"/>
-      <c r="C45" s="79"/>
-      <c r="D45" s="79"/>
-      <c r="E45" s="79"/>
-      <c r="F45" s="79"/>
+      <c r="C45" s="78"/>
+      <c r="D45" s="78"/>
+      <c r="E45" s="78"/>
+      <c r="F45" s="78"/>
       <c r="G45" s="71"/>
       <c r="H45" s="52" t="s">
         <v>68</v>
@@ -7213,14 +7218,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C39:F39"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="C4:F4"/>
@@ -7234,6 +7231,14 @@
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C39:F39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7248,7 +7253,7 @@
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="17" t="s">
@@ -7320,12 +7325,12 @@
       <c r="B4" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="85" t="s">
+      <c r="C4" s="79" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
       <c r="G4" s="40" t="s">
         <v>125</v>
       </c>
@@ -7338,12 +7343,12 @@
       <c r="B5" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="81" t="s">
+      <c r="C5" s="85" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
       <c r="G5" s="43" t="s">
         <v>121</v>
       </c>
@@ -7356,12 +7361,12 @@
       <c r="B6" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="81" t="s">
         <v>127</v>
       </c>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
       <c r="G6" s="46" t="s">
         <v>120</v>
       </c>
@@ -7455,12 +7460,12 @@
       <c r="B11" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="85" t="s">
+      <c r="C11" s="79" t="s">
         <v>128</v>
       </c>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="80"/>
       <c r="G11" s="40" t="s">
         <v>118</v>
       </c>
@@ -7473,12 +7478,12 @@
       <c r="B12" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="81" t="s">
+      <c r="C12" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="D12" s="82"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="82"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
       <c r="G12" s="43" t="s">
         <v>116</v>
       </c>
@@ -7491,12 +7496,12 @@
       <c r="B13" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="83" t="s">
+      <c r="C13" s="81" t="s">
         <v>130</v>
       </c>
-      <c r="D13" s="84"/>
-      <c r="E13" s="84"/>
-      <c r="F13" s="84"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
       <c r="G13" s="46" t="s">
         <v>120</v>
       </c>
@@ -7594,12 +7599,12 @@
       <c r="B19" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="C19" s="85" t="s">
+      <c r="C19" s="79" t="s">
         <v>131</v>
       </c>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="85"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
       <c r="G19" s="57" t="s">
         <v>122</v>
       </c>
@@ -7628,10 +7633,10 @@
     </row>
     <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="60"/>
-      <c r="C21" s="85"/>
-      <c r="D21" s="85"/>
-      <c r="E21" s="85"/>
-      <c r="F21" s="85"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="79"/>
+      <c r="E21" s="79"/>
+      <c r="F21" s="79"/>
       <c r="G21" s="60"/>
       <c r="H21" s="54" t="s">
         <v>68</v>
@@ -7721,12 +7726,12 @@
       <c r="B26" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="C26" s="85" t="s">
+      <c r="C26" s="79" t="s">
         <v>133</v>
       </c>
-      <c r="D26" s="85"/>
-      <c r="E26" s="85"/>
-      <c r="F26" s="85"/>
+      <c r="D26" s="79"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="79"/>
       <c r="G26" s="57" t="s">
         <v>125</v>
       </c>
@@ -7739,12 +7744,12 @@
       <c r="B27" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="C27" s="85" t="s">
+      <c r="C27" s="79" t="s">
         <v>135</v>
       </c>
-      <c r="D27" s="85"/>
-      <c r="E27" s="85"/>
-      <c r="F27" s="85"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="79"/>
       <c r="G27" s="58" t="s">
         <v>120</v>
       </c>
@@ -7757,12 +7762,12 @@
       <c r="B28" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="C28" s="83" t="s">
+      <c r="C28" s="81" t="s">
         <v>134</v>
       </c>
-      <c r="D28" s="83"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="83"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="81"/>
       <c r="G28" s="59" t="s">
         <v>118</v>
       </c>
@@ -7775,12 +7780,12 @@
       <c r="B29" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="C29" s="83" t="s">
+      <c r="C29" s="81" t="s">
         <v>136</v>
       </c>
-      <c r="D29" s="83"/>
-      <c r="E29" s="83"/>
-      <c r="F29" s="83"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="81"/>
       <c r="G29" s="59" t="s">
         <v>137</v>
       </c>
@@ -7809,18 +7814,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
     <mergeCell ref="C29:F29"/>
     <mergeCell ref="C27:F27"/>
     <mergeCell ref="C28:F28"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7834,7 +7839,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.5703125" style="4" customWidth="1"/>
     <col min="2" max="2" width="11" style="3" customWidth="1"/>
@@ -7972,7 +7977,7 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="9.5703125" style="3" customWidth="1"/>
@@ -8430,7 +8435,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.5703125" style="4" customWidth="1"/>
     <col min="2" max="2" width="11" style="3" customWidth="1"/>
@@ -8568,7 +8573,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="9.5703125" style="3" customWidth="1"/>
@@ -8929,7 +8934,7 @@
       <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="7.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.28515625" style="3" customWidth="1"/>
     <col min="2" max="4" width="10.28515625" style="15" customWidth="1"/>
@@ -9320,7 +9325,7 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>

</xml_diff>

<commit_message>
Se realizaron los cambios correspondientes a las horas restantes del la grafica del segundo sprint
</commit_message>
<xml_diff>
--- a/3SCRUM/Excel-Burndown-Chart-Template.xlsx
+++ b/3SCRUM/Excel-Burndown-Chart-Template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Desktop\New folder (3)\New folder\New folder (2)\New folder\New folder (2)\ProyectoMetodologia\proyectometodologia7342\3SCRUM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos de Micha\Tercer Semestre\Proyecto Metodologia\proyectometodologia7342\3SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692CF211-6F63-4151-9431-00D7AA4E544F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="4" r:id="rId1"/>
@@ -38,7 +37,7 @@
     <definedName name="WorkingDays" localSheetId="5">Sprint2Info!$B$6</definedName>
     <definedName name="WorkingDays">Sprint1Info!$B$6</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,12 +56,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>PowerUps for Excel</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -91,12 +90,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>PowerUps for Excel</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -646,7 +645,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1297,21 +1296,21 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="58">
     <dxf>
@@ -1877,7 +1876,7 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -1955,7 +1954,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Segoe UI Light"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -2493,7 +2491,7 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -2571,9 +2569,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2615,6 +2613,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2640,7 +2639,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2833,7 +2832,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -3028,7 +3027,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -3231,7 +3230,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -3247,11 +3246,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="239343728"/>
-        <c:axId val="239344120"/>
+        <c:axId val="237995584"/>
+        <c:axId val="237995976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239343728"/>
+        <c:axId val="237995584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3291,10 +3290,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239344120"/>
+        <c:crossAx val="237995976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3302,7 +3301,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239344120"/>
+        <c:axId val="237995976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3350,10 +3349,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239343728"/>
+        <c:crossAx val="237995584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3367,6 +3366,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3392,7 +3392,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3422,7 +3422,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3434,9 +3434,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3478,6 +3478,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3503,7 +3504,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3708,7 +3709,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6CB9-467B-BA08-A8BB1B63FC8E}"/>
             </c:ext>
@@ -3840,76 +3841,76 @@
                   <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91.52</c:v>
+                  <c:v>91.84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>87.039999999999992</c:v>
+                  <c:v>87.68</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82.56</c:v>
+                  <c:v>83.52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>78.08</c:v>
+                  <c:v>79.36</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>73.599999999999994</c:v>
+                  <c:v>75.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69.12</c:v>
+                  <c:v>71.039999999999992</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.64</c:v>
+                  <c:v>66.88</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>60.16</c:v>
+                  <c:v>62.72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>55.679999999999993</c:v>
+                  <c:v>58.56</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>51.199999999999996</c:v>
+                  <c:v>54.4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>46.72</c:v>
+                  <c:v>50.239999999999995</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42.239999999999995</c:v>
+                  <c:v>46.08</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>37.759999999999991</c:v>
+                  <c:v>41.92</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>33.279999999999994</c:v>
+                  <c:v>37.76</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28.799999999999997</c:v>
+                  <c:v>33.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>24.319999999999993</c:v>
+                  <c:v>29.439999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>19.839999999999989</c:v>
+                  <c:v>25.28</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>15.359999999999985</c:v>
+                  <c:v>21.120000000000005</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10.879999999999995</c:v>
+                  <c:v>16.959999999999994</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.3999999999999915</c:v>
+                  <c:v>12.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.9199999999999875</c:v>
+                  <c:v>8.64</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-2.5600000000000023</c:v>
+                  <c:v>4.4799999999999898</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6CB9-467B-BA08-A8BB1B63FC8E}"/>
             </c:ext>
@@ -4041,76 +4042,76 @@
                   <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>59</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>59</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>59</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>59</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>59</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>59</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>59</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>59</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>59</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>59</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>59</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>59</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>59</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>59</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>59</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>59</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>59</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>59</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>59</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-6CB9-467B-BA08-A8BB1B63FC8E}"/>
             </c:ext>
@@ -4126,11 +4127,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="239344904"/>
-        <c:axId val="239345296"/>
+        <c:axId val="237996760"/>
+        <c:axId val="237997152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239344904"/>
+        <c:axId val="237996760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4170,10 +4171,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239345296"/>
+        <c:crossAx val="237997152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4181,7 +4182,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239345296"/>
+        <c:axId val="237997152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4229,10 +4230,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239344904"/>
+        <c:crossAx val="237996760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4246,6 +4247,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4271,7 +4273,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4301,7 +4303,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5418,7 +5420,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5461,7 +5463,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0800-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5483,78 +5485,78 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" headerRowDxfId="55" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" headerRowDxfId="53" dataDxfId="52"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="55" dataDxfId="54"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="53" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="SprintBacklog" displayName="SprintBacklog" ref="A2:G17" totalsRowCount="1" headerRowDxfId="51" dataDxfId="50" totalsRowDxfId="49">
-  <autoFilter ref="A2:G16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SprintBacklog" displayName="SprintBacklog" ref="A2:G17" totalsRowCount="1" headerRowDxfId="51" dataDxfId="50" totalsRowDxfId="49">
+  <autoFilter ref="A2:G16"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Sprint" totalsRowLabel="1" dataDxfId="48" totalsRowDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Item ID" totalsRowFunction="custom" dataDxfId="46" totalsRowDxfId="45">
+    <tableColumn id="1" name="Sprint" totalsRowLabel="1" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="2" name="Item ID" totalsRowFunction="custom" dataDxfId="46" totalsRowDxfId="45">
       <calculatedColumnFormula>IFERROR(B2+1,1)</calculatedColumnFormula>
       <totalsRowFormula>IFERROR(B16+1,1)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Estimated Hours" totalsRowLabel="7" dataDxfId="44" totalsRowDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Task Name" totalsRowLabel="HU7-1" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Assigned To" totalsRowLabel="Emilio" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Remaining Hours" totalsRowLabel="7" dataDxfId="38" totalsRowDxfId="37">
+    <tableColumn id="3" name="Estimated Hours" totalsRowLabel="7" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="4" name="Task Name" totalsRowLabel="HU7-1" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="5" name="Assigned To" totalsRowLabel="Emilio" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="6" name="Remaining Hours" totalsRowLabel="7" dataDxfId="38" totalsRowDxfId="37">
       <calculatedColumnFormula>SprintBacklog[[#This Row],[Estimated Hours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Status" totalsRowLabel="In Progress" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="7" name="Status" totalsRowLabel="In Progress" dataDxfId="36" totalsRowDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table25" displayName="Table25" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" headerRowDxfId="32" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Column2" headerRowDxfId="30" dataDxfId="29"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="32" dataDxfId="31"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="30" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="SprintBacklog6" displayName="SprintBacklog6" ref="A2:G15" totalsRowCount="1" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="26">
-  <autoFilter ref="A2:G14" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="SprintBacklog6" displayName="SprintBacklog6" ref="A2:G15" totalsRowCount="1" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="26">
+  <autoFilter ref="A2:G14"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Sprint" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Item ID" dataDxfId="23" totalsRowDxfId="22">
+    <tableColumn id="1" name="Sprint" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" name="Item ID" dataDxfId="23" totalsRowDxfId="22">
       <calculatedColumnFormula>IFERROR(B2+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Task Name" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Assigned To" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Remaining Hours" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14">
+    <tableColumn id="3" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" name="Task Name" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" name="Assigned To" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" name="Remaining Hours" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14">
       <calculatedColumnFormula>SprintBacklog6[[#This Row],[Estimated Hours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Status" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="7" name="Status" dataDxfId="13" totalsRowDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table3" displayName="Table3" ref="A2:D23" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A2:D23" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:D23" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A2:D23"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Work Day" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Target Burn Down" dataDxfId="8">
+    <tableColumn id="1" name="Work Day" dataDxfId="9"/>
+    <tableColumn id="2" name="Target Burn Down" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(Target-(Table3[[#This Row],[Work Day]]*(Target/WorkingDays)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Forecast Burn Down" dataDxfId="7">
+    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="7">
       <calculatedColumnFormula>Target-(Table3[[#This Row],[Work Day]]*DevRate)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Actual Burn Down" dataDxfId="6">
+    <tableColumn id="4" name="Actual Burn Down" dataDxfId="6">
       <calculatedColumnFormula>Table3[[#This Row],[Target Burn Down]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5563,17 +5565,17 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table38" displayName="Table38" ref="A2:D25" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A2:D25" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table38" displayName="Table38" ref="A2:D25" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A2:D25"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Work Day" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Target Burn Down" dataDxfId="2">
+    <tableColumn id="1" name="Work Day" dataDxfId="3"/>
+    <tableColumn id="2" name="Target Burn Down" dataDxfId="2">
       <calculatedColumnFormula>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Forecast Burn Down" dataDxfId="1">
+    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="1">
       <calculatedColumnFormula>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Actual Burn Down" dataDxfId="0"/>
+    <tableColumn id="4" name="Actual Burn Down" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5841,14 +5843,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="31.7109375" customWidth="1"/>
     <col min="5" max="5" width="63.85546875" customWidth="1"/>
@@ -6225,14 +6227,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="30.7109375" customWidth="1"/>
     <col min="6" max="6" width="35.42578125" customWidth="1"/>
@@ -6312,12 +6314,12 @@
       <c r="B4" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="85" t="s">
+      <c r="C4" s="81" t="s">
         <v>115</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
       <c r="G4" s="43" t="s">
         <v>121</v>
       </c>
@@ -6331,12 +6333,12 @@
       <c r="B5" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="81" t="s">
+      <c r="C5" s="83" t="s">
         <v>154</v>
       </c>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
       <c r="G5" s="46" t="s">
         <v>116</v>
       </c>
@@ -6348,10 +6350,10 @@
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
       <c r="G6" s="18"/>
       <c r="H6" s="52" t="s">
         <v>68</v>
@@ -6435,12 +6437,12 @@
       <c r="B10" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="79" t="s">
+      <c r="C10" s="85" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
       <c r="G10" s="40" t="s">
         <v>118</v>
       </c>
@@ -6454,12 +6456,12 @@
       <c r="B11" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="85" t="s">
+      <c r="C11" s="81" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
       <c r="G11" s="43" t="s">
         <v>116</v>
       </c>
@@ -6473,12 +6475,12 @@
       <c r="B12" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="81" t="s">
+      <c r="C12" s="83" t="s">
         <v>155</v>
       </c>
-      <c r="D12" s="82"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="82"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84"/>
       <c r="G12" s="46" t="s">
         <v>120</v>
       </c>
@@ -6490,10 +6492,10 @@
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="18"/>
-      <c r="C13" s="78"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="79"/>
       <c r="G13" s="18"/>
       <c r="H13" s="52" t="s">
         <v>68</v>
@@ -6577,12 +6579,12 @@
       <c r="B17" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="79" t="s">
+      <c r="C17" s="85" t="s">
         <v>156</v>
       </c>
-      <c r="D17" s="80"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
       <c r="G17" s="40" t="s">
         <v>122</v>
       </c>
@@ -6596,12 +6598,12 @@
       <c r="B18" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="85" t="s">
+      <c r="C18" s="81" t="s">
         <v>157</v>
       </c>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="82"/>
       <c r="G18" s="43" t="s">
         <v>118</v>
       </c>
@@ -6615,12 +6617,12 @@
       <c r="B19" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="81" t="s">
+      <c r="C19" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="D19" s="82"/>
-      <c r="E19" s="82"/>
-      <c r="F19" s="82"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="84"/>
       <c r="G19" s="46" t="s">
         <v>116</v>
       </c>
@@ -6719,12 +6721,12 @@
       <c r="B24" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="79" t="s">
+      <c r="C24" s="85" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="80"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
       <c r="G24" s="40" t="s">
         <v>120</v>
       </c>
@@ -6738,12 +6740,12 @@
       <c r="B25" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="84" t="s">
+      <c r="C25" s="80" t="s">
         <v>138</v>
       </c>
-      <c r="D25" s="84"/>
-      <c r="E25" s="84"/>
-      <c r="F25" s="84"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
       <c r="G25" s="46" t="s">
         <v>121</v>
       </c>
@@ -6755,10 +6757,10 @@
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="18"/>
-      <c r="C26" s="83"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="78"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="79"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="79"/>
       <c r="G26" s="18"/>
       <c r="H26" s="52" t="s">
         <v>68</v>
@@ -6853,12 +6855,12 @@
       <c r="B31" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="79" t="s">
+      <c r="C31" s="85" t="s">
         <v>159</v>
       </c>
-      <c r="D31" s="80"/>
-      <c r="E31" s="80"/>
-      <c r="F31" s="80"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="86"/>
       <c r="G31" s="40" t="s">
         <v>116</v>
       </c>
@@ -6872,12 +6874,12 @@
       <c r="B32" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="81" t="s">
+      <c r="C32" s="83" t="s">
         <v>160</v>
       </c>
-      <c r="D32" s="82"/>
-      <c r="E32" s="82"/>
-      <c r="F32" s="82"/>
+      <c r="D32" s="84"/>
+      <c r="E32" s="84"/>
+      <c r="F32" s="84"/>
       <c r="G32" s="46" t="s">
         <v>120</v>
       </c>
@@ -6976,12 +6978,12 @@
       <c r="B37" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="79" t="s">
+      <c r="C37" s="85" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="80"/>
-      <c r="E37" s="80"/>
-      <c r="F37" s="80"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="86"/>
       <c r="G37" s="40" t="s">
         <v>118</v>
       </c>
@@ -6995,12 +6997,12 @@
       <c r="B38" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="81" t="s">
+      <c r="C38" s="83" t="s">
         <v>162</v>
       </c>
-      <c r="D38" s="82"/>
-      <c r="E38" s="82"/>
-      <c r="F38" s="82"/>
+      <c r="D38" s="84"/>
+      <c r="E38" s="84"/>
+      <c r="F38" s="84"/>
       <c r="G38" s="46" t="s">
         <v>122</v>
       </c>
@@ -7012,10 +7014,10 @@
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19"/>
       <c r="B39" s="18"/>
-      <c r="C39" s="78"/>
-      <c r="D39" s="78"/>
-      <c r="E39" s="78"/>
-      <c r="F39" s="78"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="79"/>
+      <c r="E39" s="79"/>
+      <c r="F39" s="79"/>
       <c r="G39" s="18"/>
       <c r="H39" s="52" t="s">
         <v>68</v>
@@ -7099,12 +7101,12 @@
       <c r="B43" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="C43" s="79" t="s">
+      <c r="C43" s="85" t="s">
         <v>163</v>
       </c>
-      <c r="D43" s="80"/>
-      <c r="E43" s="80"/>
-      <c r="F43" s="80"/>
+      <c r="D43" s="86"/>
+      <c r="E43" s="86"/>
+      <c r="F43" s="86"/>
       <c r="G43" s="69" t="s">
         <v>118</v>
       </c>
@@ -7118,12 +7120,12 @@
       <c r="B44" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="81" t="s">
+      <c r="C44" s="83" t="s">
         <v>164</v>
       </c>
-      <c r="D44" s="82"/>
-      <c r="E44" s="82"/>
-      <c r="F44" s="82"/>
+      <c r="D44" s="84"/>
+      <c r="E44" s="84"/>
+      <c r="F44" s="84"/>
       <c r="G44" s="70" t="s">
         <v>116</v>
       </c>
@@ -7135,10 +7137,10 @@
     <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19"/>
       <c r="B45" s="71"/>
-      <c r="C45" s="78"/>
-      <c r="D45" s="78"/>
-      <c r="E45" s="78"/>
-      <c r="F45" s="78"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="79"/>
+      <c r="E45" s="79"/>
+      <c r="F45" s="79"/>
       <c r="G45" s="71"/>
       <c r="H45" s="52" t="s">
         <v>68</v>
@@ -7218,6 +7220,14 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C39:F39"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="C4:F4"/>
@@ -7231,14 +7241,6 @@
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C39:F39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7246,14 +7248,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="17" t="s">
@@ -7325,12 +7327,12 @@
       <c r="B4" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="79" t="s">
+      <c r="C4" s="85" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="40" t="s">
         <v>125</v>
       </c>
@@ -7343,12 +7345,12 @@
       <c r="B5" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="81" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
       <c r="G5" s="43" t="s">
         <v>121</v>
       </c>
@@ -7361,12 +7363,12 @@
       <c r="B6" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="81" t="s">
+      <c r="C6" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
       <c r="G6" s="46" t="s">
         <v>120</v>
       </c>
@@ -7460,12 +7462,12 @@
       <c r="B11" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="79" t="s">
+      <c r="C11" s="85" t="s">
         <v>128</v>
       </c>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
       <c r="G11" s="40" t="s">
         <v>118</v>
       </c>
@@ -7478,12 +7480,12 @@
       <c r="B12" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="85" t="s">
+      <c r="C12" s="81" t="s">
         <v>129</v>
       </c>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
       <c r="G12" s="43" t="s">
         <v>116</v>
       </c>
@@ -7496,12 +7498,12 @@
       <c r="B13" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="81" t="s">
+      <c r="C13" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="84"/>
       <c r="G13" s="46" t="s">
         <v>120</v>
       </c>
@@ -7599,12 +7601,12 @@
       <c r="B19" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="C19" s="79" t="s">
+      <c r="C19" s="85" t="s">
         <v>131</v>
       </c>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="79"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
       <c r="G19" s="57" t="s">
         <v>122</v>
       </c>
@@ -7633,10 +7635,10 @@
     </row>
     <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="60"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="79"/>
-      <c r="F21" s="79"/>
+      <c r="C21" s="85"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="85"/>
+      <c r="F21" s="85"/>
       <c r="G21" s="60"/>
       <c r="H21" s="54" t="s">
         <v>68</v>
@@ -7726,12 +7728,12 @@
       <c r="B26" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="C26" s="79" t="s">
+      <c r="C26" s="85" t="s">
         <v>133</v>
       </c>
-      <c r="D26" s="79"/>
-      <c r="E26" s="79"/>
-      <c r="F26" s="79"/>
+      <c r="D26" s="85"/>
+      <c r="E26" s="85"/>
+      <c r="F26" s="85"/>
       <c r="G26" s="57" t="s">
         <v>125</v>
       </c>
@@ -7744,12 +7746,12 @@
       <c r="B27" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="C27" s="79" t="s">
+      <c r="C27" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="79"/>
+      <c r="D27" s="85"/>
+      <c r="E27" s="85"/>
+      <c r="F27" s="85"/>
       <c r="G27" s="58" t="s">
         <v>120</v>
       </c>
@@ -7762,12 +7764,12 @@
       <c r="B28" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="C28" s="81" t="s">
+      <c r="C28" s="83" t="s">
         <v>134</v>
       </c>
-      <c r="D28" s="81"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81"/>
+      <c r="D28" s="83"/>
+      <c r="E28" s="83"/>
+      <c r="F28" s="83"/>
       <c r="G28" s="59" t="s">
         <v>118</v>
       </c>
@@ -7780,12 +7782,12 @@
       <c r="B29" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="C29" s="81" t="s">
+      <c r="C29" s="83" t="s">
         <v>136</v>
       </c>
-      <c r="D29" s="81"/>
-      <c r="E29" s="81"/>
-      <c r="F29" s="81"/>
+      <c r="D29" s="83"/>
+      <c r="E29" s="83"/>
+      <c r="F29" s="83"/>
       <c r="G29" s="59" t="s">
         <v>137</v>
       </c>
@@ -7814,32 +7816,32 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C26:F26"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C26:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.5703125" style="4" customWidth="1"/>
     <col min="2" max="2" width="11" style="3" customWidth="1"/>
@@ -7970,14 +7972,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="9.5703125" style="3" customWidth="1"/>
@@ -8416,7 +8418,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G16 G18" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G16 G18">
       <formula1>"In Progress, Completed, Blocked"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8428,14 +8430,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.5703125" style="4" customWidth="1"/>
     <col min="2" max="2" width="11" style="3" customWidth="1"/>
@@ -8509,7 +8511,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="8">
-        <v>0.14000000000000001</v>
+        <v>0.13</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -8521,7 +8523,7 @@
       </c>
       <c r="B9" s="3">
         <f>(B4-B5)*B8*B7*8</f>
-        <v>98.56</v>
+        <v>91.52000000000001</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -8531,7 +8533,7 @@
       </c>
       <c r="B10" s="3">
         <f>IFERROR(B9/B4,0)</f>
-        <v>4.4800000000000004</v>
+        <v>4.16</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -8566,14 +8568,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G15"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="9.5703125" style="3" customWidth="1"/>
@@ -8915,7 +8917,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G14" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G14">
       <formula1>"In Progress, Completed, Blocked"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8927,14 +8929,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.28515625" style="3" customWidth="1"/>
     <col min="2" max="4" width="10.28515625" style="15" customWidth="1"/>
@@ -9318,14 +9320,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
@@ -9410,10 +9412,10 @@
       </c>
       <c r="C4" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>91.52</v>
+        <v>91.84</v>
       </c>
       <c r="D4" s="16">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="3"/>
@@ -9438,10 +9440,10 @@
       </c>
       <c r="C5" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>87.039999999999992</v>
+        <v>87.68</v>
       </c>
       <c r="D5" s="16">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="3"/>
@@ -9466,10 +9468,10 @@
       </c>
       <c r="C6" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>82.56</v>
+        <v>83.52</v>
       </c>
       <c r="D6" s="16">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="3"/>
@@ -9494,10 +9496,10 @@
       </c>
       <c r="C7" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>78.08</v>
+        <v>79.36</v>
       </c>
       <c r="D7" s="16">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="3"/>
@@ -9522,10 +9524,10 @@
       </c>
       <c r="C8" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>73.599999999999994</v>
+        <v>75.2</v>
       </c>
       <c r="D8" s="16">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="3"/>
@@ -9550,10 +9552,10 @@
       </c>
       <c r="C9" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>69.12</v>
+        <v>71.039999999999992</v>
       </c>
       <c r="D9" s="16">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="3"/>
@@ -9578,10 +9580,10 @@
       </c>
       <c r="C10" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>64.64</v>
+        <v>66.88</v>
       </c>
       <c r="D10" s="16">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="3"/>
@@ -9606,10 +9608,10 @@
       </c>
       <c r="C11" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>60.16</v>
+        <v>62.72</v>
       </c>
       <c r="D11" s="16">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="3"/>
@@ -9634,7 +9636,7 @@
       </c>
       <c r="C12" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>55.679999999999993</v>
+        <v>58.56</v>
       </c>
       <c r="D12" s="16">
         <v>59</v>
@@ -9662,10 +9664,10 @@
       </c>
       <c r="C13" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>51.199999999999996</v>
+        <v>54.4</v>
       </c>
       <c r="D13" s="16">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="3"/>
@@ -9690,10 +9692,10 @@
       </c>
       <c r="C14" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>46.72</v>
+        <v>50.239999999999995</v>
       </c>
       <c r="D14" s="16">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -9718,10 +9720,10 @@
       </c>
       <c r="C15" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>42.239999999999995</v>
+        <v>46.08</v>
       </c>
       <c r="D15" s="16">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -9746,10 +9748,10 @@
       </c>
       <c r="C16" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>37.759999999999991</v>
+        <v>41.92</v>
       </c>
       <c r="D16" s="16">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9762,10 +9764,10 @@
       </c>
       <c r="C17" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>33.279999999999994</v>
+        <v>37.76</v>
       </c>
       <c r="D17" s="16">
-        <v>59</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9778,10 +9780,10 @@
       </c>
       <c r="C18" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>28.799999999999997</v>
+        <v>33.599999999999994</v>
       </c>
       <c r="D18" s="16">
-        <v>59</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9794,10 +9796,10 @@
       </c>
       <c r="C19" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>24.319999999999993</v>
+        <v>29.439999999999998</v>
       </c>
       <c r="D19" s="16">
-        <v>59</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9810,10 +9812,10 @@
       </c>
       <c r="C20" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>19.839999999999989</v>
+        <v>25.28</v>
       </c>
       <c r="D20" s="16">
-        <v>59</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9826,10 +9828,10 @@
       </c>
       <c r="C21" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>15.359999999999985</v>
+        <v>21.120000000000005</v>
       </c>
       <c r="D21" s="16">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9842,10 +9844,10 @@
       </c>
       <c r="C22" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>10.879999999999995</v>
+        <v>16.959999999999994</v>
       </c>
       <c r="D22" s="16">
-        <v>59</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9858,10 +9860,10 @@
       </c>
       <c r="C23" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>6.3999999999999915</v>
+        <v>12.799999999999997</v>
       </c>
       <c r="D23" s="16">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9874,10 +9876,10 @@
       </c>
       <c r="C24" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>1.9199999999999875</v>
+        <v>8.64</v>
       </c>
       <c r="D24" s="16">
-        <v>59</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9890,10 +9892,10 @@
       </c>
       <c r="C25" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>-2.5600000000000023</v>
+        <v>4.4799999999999898</v>
       </c>
       <c r="D25" s="16">
-        <v>59</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se asignaron las horas restantes corespondientes al sprint2, ademas queda correjido la aparicion de valores negativos en la grafica
</commit_message>
<xml_diff>
--- a/3SCRUM/Excel-Burndown-Chart-Template.xlsx
+++ b/3SCRUM/Excel-Burndown-Chart-Template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emili\Desktop\ProyectoMetodologia\proyectometodologia7342\proyectometodologia7342\3SCRUM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos de Micha\Tercer Semestre\Proyecto Metodologia\proyectometodologia7342\3SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD58E93-EE00-4F1D-9642-DDAD5AF981DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="4" r:id="rId1"/>
@@ -38,7 +37,7 @@
     <definedName name="WorkingDays" localSheetId="5">Sprint2Info!$B$6</definedName>
     <definedName name="WorkingDays">Sprint1Info!$B$6</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -55,12 +54,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>PowerUps for Excel</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -89,12 +88,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>PowerUps for Excel</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -626,7 +625,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1277,17 +1276,17 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1935,7 +1934,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Segoe UI Light"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -2551,7 +2549,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -2595,6 +2593,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2620,7 +2619,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-EC"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2813,7 +2812,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -3008,7 +3007,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -3211,7 +3210,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -3227,11 +3226,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="239343728"/>
-        <c:axId val="239344120"/>
+        <c:axId val="228843752"/>
+        <c:axId val="228845320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239343728"/>
+        <c:axId val="228843752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3271,10 +3270,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-EC"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239344120"/>
+        <c:crossAx val="228845320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3282,7 +3281,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239344120"/>
+        <c:axId val="228845320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3330,10 +3329,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-EC"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239343728"/>
+        <c:crossAx val="228843752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3347,6 +3346,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3372,7 +3372,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-EC"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3402,7 +3402,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-EC"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3414,7 +3414,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -3458,6 +3458,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3483,7 +3484,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-EC"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3688,7 +3689,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6CB9-467B-BA08-A8BB1B63FC8E}"/>
             </c:ext>
@@ -3820,76 +3821,76 @@
                   <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91.52</c:v>
+                  <c:v>91.84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>87.039999999999992</c:v>
+                  <c:v>87.68</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82.56</c:v>
+                  <c:v>83.52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>78.08</c:v>
+                  <c:v>79.36</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>73.599999999999994</c:v>
+                  <c:v>75.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69.12</c:v>
+                  <c:v>71.039999999999992</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.64</c:v>
+                  <c:v>66.88</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>60.16</c:v>
+                  <c:v>62.72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>55.679999999999993</c:v>
+                  <c:v>58.56</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>51.199999999999996</c:v>
+                  <c:v>54.4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>46.72</c:v>
+                  <c:v>50.239999999999995</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42.239999999999995</c:v>
+                  <c:v>46.08</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>37.759999999999991</c:v>
+                  <c:v>41.92</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>33.279999999999994</c:v>
+                  <c:v>37.76</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28.799999999999997</c:v>
+                  <c:v>33.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>24.319999999999993</c:v>
+                  <c:v>29.439999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>19.839999999999989</c:v>
+                  <c:v>25.28</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>15.359999999999985</c:v>
+                  <c:v>21.120000000000005</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10.879999999999995</c:v>
+                  <c:v>16.959999999999994</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.3999999999999915</c:v>
+                  <c:v>12.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.9199999999999875</c:v>
+                  <c:v>8.64</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-2.5600000000000023</c:v>
+                  <c:v>4.4799999999999898</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6CB9-467B-BA08-A8BB1B63FC8E}"/>
             </c:ext>
@@ -4021,76 +4022,76 @@
                   <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>59</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>59</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>59</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>59</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>59</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>59</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>59</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>59</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>59</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>59</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>59</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>59</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>59</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>59</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>59</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>59</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>59</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>59</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>59</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>59</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-6CB9-467B-BA08-A8BB1B63FC8E}"/>
             </c:ext>
@@ -4106,11 +4107,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="239344904"/>
-        <c:axId val="239345296"/>
+        <c:axId val="229436832"/>
+        <c:axId val="228498392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239344904"/>
+        <c:axId val="229436832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4150,10 +4151,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-EC"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239345296"/>
+        <c:crossAx val="228498392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4161,7 +4162,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239345296"/>
+        <c:axId val="228498392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4209,10 +4210,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-EC"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239344904"/>
+        <c:crossAx val="229436832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4226,6 +4227,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4251,7 +4253,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-EC"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4281,7 +4283,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-EC"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5398,7 +5400,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5441,7 +5443,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0800-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5463,78 +5465,78 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" headerRowDxfId="55" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" headerRowDxfId="53" dataDxfId="52"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="55" dataDxfId="54"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="53" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="SprintBacklog" displayName="SprintBacklog" ref="A2:G17" totalsRowCount="1" headerRowDxfId="51" dataDxfId="50" totalsRowDxfId="49">
-  <autoFilter ref="A2:G16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SprintBacklog" displayName="SprintBacklog" ref="A2:G17" totalsRowCount="1" headerRowDxfId="51" dataDxfId="50" totalsRowDxfId="49">
+  <autoFilter ref="A2:G16"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Sprint" totalsRowLabel="1" dataDxfId="48" totalsRowDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Item ID" totalsRowFunction="custom" dataDxfId="46" totalsRowDxfId="45">
+    <tableColumn id="1" name="Sprint" totalsRowLabel="1" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="2" name="Item ID" totalsRowFunction="custom" dataDxfId="46" totalsRowDxfId="45">
       <calculatedColumnFormula>IFERROR(B2+1,1)</calculatedColumnFormula>
       <totalsRowFormula>IFERROR(B16+1,1)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Estimated Hours" totalsRowLabel="7" dataDxfId="44" totalsRowDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Task Name" totalsRowLabel="HU7-1" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Assigned To" totalsRowLabel="Emilio" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Remaining Hours" totalsRowLabel="7" dataDxfId="38" totalsRowDxfId="37">
+    <tableColumn id="3" name="Estimated Hours" totalsRowLabel="7" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="4" name="Task Name" totalsRowLabel="HU7-1" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="5" name="Assigned To" totalsRowLabel="Emilio" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="6" name="Remaining Hours" totalsRowLabel="7" dataDxfId="38" totalsRowDxfId="37">
       <calculatedColumnFormula>SprintBacklog[[#This Row],[Estimated Hours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Status" totalsRowLabel="In Progress" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="7" name="Status" totalsRowLabel="In Progress" dataDxfId="36" totalsRowDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table25" displayName="Table25" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" headerRowDxfId="32" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Column2" headerRowDxfId="30" dataDxfId="29"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="32" dataDxfId="31"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="30" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="SprintBacklog6" displayName="SprintBacklog6" ref="A2:G15" totalsRowCount="1" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="26">
-  <autoFilter ref="A2:G14" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="SprintBacklog6" displayName="SprintBacklog6" ref="A2:G15" totalsRowCount="1" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="26">
+  <autoFilter ref="A2:G14"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Sprint" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Item ID" dataDxfId="23" totalsRowDxfId="22">
+    <tableColumn id="1" name="Sprint" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" name="Item ID" dataDxfId="23" totalsRowDxfId="22">
       <calculatedColumnFormula>IFERROR(B2+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Task Name" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Assigned To" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Remaining Hours" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14">
+    <tableColumn id="3" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" name="Task Name" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" name="Assigned To" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" name="Remaining Hours" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14">
       <calculatedColumnFormula>SprintBacklog6[[#This Row],[Estimated Hours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Status" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="7" name="Status" dataDxfId="13" totalsRowDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table3" displayName="Table3" ref="A2:D23" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A2:D23" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:D23" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A2:D23"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Work Day" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Target Burn Down" dataDxfId="8">
+    <tableColumn id="1" name="Work Day" dataDxfId="9"/>
+    <tableColumn id="2" name="Target Burn Down" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(Target-(Table3[[#This Row],[Work Day]]*(Target/WorkingDays)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Forecast Burn Down" dataDxfId="7">
+    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="7">
       <calculatedColumnFormula>Target-(Table3[[#This Row],[Work Day]]*DevRate)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Actual Burn Down" dataDxfId="6">
+    <tableColumn id="4" name="Actual Burn Down" dataDxfId="6">
       <calculatedColumnFormula>Table3[[#This Row],[Target Burn Down]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5543,17 +5545,17 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table38" displayName="Table38" ref="A2:D25" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A2:D25" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table38" displayName="Table38" ref="A2:D25" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A2:D25"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Work Day" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Target Burn Down" dataDxfId="2">
+    <tableColumn id="1" name="Work Day" dataDxfId="3"/>
+    <tableColumn id="2" name="Target Burn Down" dataDxfId="2">
       <calculatedColumnFormula>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Forecast Burn Down" dataDxfId="1">
+    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="1">
       <calculatedColumnFormula>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Actual Burn Down" dataDxfId="0"/>
+    <tableColumn id="4" name="Actual Burn Down" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5821,7 +5823,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -6189,7 +6191,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -6276,12 +6278,12 @@
       <c r="B4" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="43" t="s">
         <v>107</v>
       </c>
@@ -6295,12 +6297,12 @@
       <c r="B5" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="81" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
       <c r="G5" s="46" t="s">
         <v>102</v>
       </c>
@@ -6312,10 +6314,10 @@
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
       <c r="G6" s="18"/>
       <c r="H6" s="52" t="s">
         <v>58</v>
@@ -6399,12 +6401,12 @@
       <c r="B10" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="85" t="s">
+      <c r="C10" s="79" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
       <c r="G10" s="40" t="s">
         <v>104</v>
       </c>
@@ -6418,12 +6420,12 @@
       <c r="B11" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="81" t="s">
+      <c r="C11" s="85" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="82"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
       <c r="G11" s="43" t="s">
         <v>102</v>
       </c>
@@ -6437,12 +6439,12 @@
       <c r="B12" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="83" t="s">
+      <c r="C12" s="81" t="s">
         <v>133</v>
       </c>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
       <c r="G12" s="46" t="s">
         <v>106</v>
       </c>
@@ -6454,10 +6456,10 @@
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="18"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="79"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="79"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
       <c r="G13" s="18"/>
       <c r="H13" s="52" t="s">
         <v>58</v>
@@ -6541,12 +6543,12 @@
       <c r="B17" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="85" t="s">
+      <c r="C17" s="79" t="s">
         <v>134</v>
       </c>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80"/>
       <c r="G17" s="40" t="s">
         <v>108</v>
       </c>
@@ -6560,12 +6562,12 @@
       <c r="B18" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="81" t="s">
+      <c r="C18" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="82"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
       <c r="G18" s="43" t="s">
         <v>104</v>
       </c>
@@ -6579,12 +6581,12 @@
       <c r="B19" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="83" t="s">
+      <c r="C19" s="81" t="s">
         <v>136</v>
       </c>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="84"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
       <c r="G19" s="46" t="s">
         <v>102</v>
       </c>
@@ -6683,12 +6685,12 @@
       <c r="B24" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="85" t="s">
+      <c r="C24" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
       <c r="G24" s="40" t="s">
         <v>106</v>
       </c>
@@ -6702,12 +6704,12 @@
       <c r="B25" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="80" t="s">
+      <c r="C25" s="84" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="84"/>
       <c r="G25" s="46" t="s">
         <v>107</v>
       </c>
@@ -6719,10 +6721,10 @@
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="18"/>
-      <c r="C26" s="78"/>
-      <c r="D26" s="79"/>
-      <c r="E26" s="79"/>
-      <c r="F26" s="79"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
       <c r="G26" s="18"/>
       <c r="H26" s="52" t="s">
         <v>58</v>
@@ -6817,12 +6819,12 @@
       <c r="B31" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="85" t="s">
+      <c r="C31" s="79" t="s">
         <v>137</v>
       </c>
-      <c r="D31" s="86"/>
-      <c r="E31" s="86"/>
-      <c r="F31" s="86"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="80"/>
       <c r="G31" s="40" t="s">
         <v>102</v>
       </c>
@@ -6836,12 +6838,12 @@
       <c r="B32" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="83" t="s">
+      <c r="C32" s="81" t="s">
         <v>138</v>
       </c>
-      <c r="D32" s="84"/>
-      <c r="E32" s="84"/>
-      <c r="F32" s="84"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="82"/>
       <c r="G32" s="46" t="s">
         <v>106</v>
       </c>
@@ -6940,12 +6942,12 @@
       <c r="B37" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="85" t="s">
+      <c r="C37" s="79" t="s">
         <v>139</v>
       </c>
-      <c r="D37" s="86"/>
-      <c r="E37" s="86"/>
-      <c r="F37" s="86"/>
+      <c r="D37" s="80"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="80"/>
       <c r="G37" s="40" t="s">
         <v>104</v>
       </c>
@@ -6959,12 +6961,12 @@
       <c r="B38" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="83" t="s">
+      <c r="C38" s="81" t="s">
         <v>140</v>
       </c>
-      <c r="D38" s="84"/>
-      <c r="E38" s="84"/>
-      <c r="F38" s="84"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="82"/>
       <c r="G38" s="46" t="s">
         <v>108</v>
       </c>
@@ -6976,10 +6978,10 @@
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19"/>
       <c r="B39" s="18"/>
-      <c r="C39" s="79"/>
-      <c r="D39" s="79"/>
-      <c r="E39" s="79"/>
-      <c r="F39" s="79"/>
+      <c r="C39" s="78"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="78"/>
       <c r="G39" s="18"/>
       <c r="H39" s="52" t="s">
         <v>58</v>
@@ -7063,12 +7065,12 @@
       <c r="B43" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="85" t="s">
+      <c r="C43" s="79" t="s">
         <v>141</v>
       </c>
-      <c r="D43" s="86"/>
-      <c r="E43" s="86"/>
-      <c r="F43" s="86"/>
+      <c r="D43" s="80"/>
+      <c r="E43" s="80"/>
+      <c r="F43" s="80"/>
       <c r="G43" s="69" t="s">
         <v>104</v>
       </c>
@@ -7082,12 +7084,12 @@
       <c r="B44" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="83" t="s">
+      <c r="C44" s="81" t="s">
         <v>142</v>
       </c>
-      <c r="D44" s="84"/>
-      <c r="E44" s="84"/>
-      <c r="F44" s="84"/>
+      <c r="D44" s="82"/>
+      <c r="E44" s="82"/>
+      <c r="F44" s="82"/>
       <c r="G44" s="70" t="s">
         <v>102</v>
       </c>
@@ -7099,10 +7101,10 @@
     <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19"/>
       <c r="B45" s="71"/>
-      <c r="C45" s="79"/>
-      <c r="D45" s="79"/>
-      <c r="E45" s="79"/>
-      <c r="F45" s="79"/>
+      <c r="C45" s="78"/>
+      <c r="D45" s="78"/>
+      <c r="E45" s="78"/>
+      <c r="F45" s="78"/>
       <c r="G45" s="71"/>
       <c r="H45" s="52" t="s">
         <v>58</v>
@@ -7182,14 +7184,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C39:F39"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="C4:F4"/>
@@ -7203,6 +7197,14 @@
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C39:F39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7210,7 +7212,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -7293,12 +7295,12 @@
       <c r="B4" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="85" t="s">
+      <c r="C4" s="79" t="s">
         <v>155</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
       <c r="G4" s="40" t="s">
         <v>110</v>
       </c>
@@ -7311,12 +7313,12 @@
       <c r="B5" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="81" t="s">
+      <c r="C5" s="85" t="s">
         <v>156</v>
       </c>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
       <c r="G5" s="43" t="s">
         <v>107</v>
       </c>
@@ -7329,12 +7331,12 @@
       <c r="B6" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="81" t="s">
         <v>157</v>
       </c>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
       <c r="G6" s="46" t="s">
         <v>106</v>
       </c>
@@ -7428,12 +7430,12 @@
       <c r="B11" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="C11" s="85" t="s">
+      <c r="C11" s="79" t="s">
         <v>160</v>
       </c>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="80"/>
       <c r="G11" s="40" t="s">
         <v>104</v>
       </c>
@@ -7446,12 +7448,12 @@
       <c r="B12" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="81" t="s">
+      <c r="C12" s="85" t="s">
         <v>161</v>
       </c>
-      <c r="D12" s="82"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="82"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
       <c r="G12" s="43" t="s">
         <v>102</v>
       </c>
@@ -7464,12 +7466,12 @@
       <c r="B13" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="C13" s="83" t="s">
+      <c r="C13" s="81" t="s">
         <v>162</v>
       </c>
-      <c r="D13" s="84"/>
-      <c r="E13" s="84"/>
-      <c r="F13" s="84"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
       <c r="G13" s="46" t="s">
         <v>106</v>
       </c>
@@ -7567,12 +7569,12 @@
       <c r="B19" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="C19" s="85" t="s">
+      <c r="C19" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="85"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
       <c r="G19" s="57" t="s">
         <v>108</v>
       </c>
@@ -7601,10 +7603,10 @@
     </row>
     <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="60"/>
-      <c r="C21" s="85"/>
-      <c r="D21" s="85"/>
-      <c r="E21" s="85"/>
-      <c r="F21" s="85"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="79"/>
+      <c r="E21" s="79"/>
+      <c r="F21" s="79"/>
       <c r="G21" s="60"/>
       <c r="H21" s="54" t="s">
         <v>58</v>
@@ -7694,12 +7696,12 @@
       <c r="B26" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="C26" s="85" t="s">
+      <c r="C26" s="79" t="s">
         <v>111</v>
       </c>
-      <c r="D26" s="85"/>
-      <c r="E26" s="85"/>
-      <c r="F26" s="85"/>
+      <c r="D26" s="79"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="79"/>
       <c r="G26" s="57" t="s">
         <v>110</v>
       </c>
@@ -7712,12 +7714,12 @@
       <c r="B27" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="C27" s="85" t="s">
+      <c r="C27" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="85"/>
-      <c r="E27" s="85"/>
-      <c r="F27" s="85"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="79"/>
       <c r="G27" s="58" t="s">
         <v>106</v>
       </c>
@@ -7730,12 +7732,12 @@
       <c r="B28" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="C28" s="83" t="s">
+      <c r="C28" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="D28" s="83"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="83"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="81"/>
       <c r="G28" s="59" t="s">
         <v>104</v>
       </c>
@@ -7748,12 +7750,12 @@
       <c r="B29" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="C29" s="83" t="s">
+      <c r="C29" s="81" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="83"/>
-      <c r="E29" s="83"/>
-      <c r="F29" s="83"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="81"/>
       <c r="G29" s="59" t="s">
         <v>115</v>
       </c>
@@ -7782,25 +7784,25 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
     <mergeCell ref="C29:F29"/>
     <mergeCell ref="C27:F27"/>
     <mergeCell ref="C28:F28"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
@@ -7938,7 +7940,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -8384,7 +8386,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G16 G18" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G16 G18">
       <formula1>"In Progress, Completed, Blocked"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8396,11 +8398,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8477,7 +8479,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="8">
-        <v>0.14000000000000001</v>
+        <v>0.13</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -8489,7 +8491,7 @@
       </c>
       <c r="B9" s="3">
         <f>(B4-B5)*B8*B7*8</f>
-        <v>98.56</v>
+        <v>91.52000000000001</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -8499,7 +8501,7 @@
       </c>
       <c r="B10" s="3">
         <f>IFERROR(B9/B4,0)</f>
-        <v>4.4800000000000004</v>
+        <v>4.16</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -8534,10 +8536,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -8883,7 +8885,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G14" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G14">
       <formula1>"In Progress, Completed, Blocked"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8895,7 +8897,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E23"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -9286,11 +9288,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9378,10 +9380,10 @@
       </c>
       <c r="C4" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>91.52</v>
+        <v>91.84</v>
       </c>
       <c r="D4" s="16">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="3"/>
@@ -9406,10 +9408,10 @@
       </c>
       <c r="C5" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>87.039999999999992</v>
+        <v>87.68</v>
       </c>
       <c r="D5" s="16">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="3"/>
@@ -9434,10 +9436,10 @@
       </c>
       <c r="C6" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>82.56</v>
+        <v>83.52</v>
       </c>
       <c r="D6" s="16">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="3"/>
@@ -9462,10 +9464,10 @@
       </c>
       <c r="C7" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>78.08</v>
+        <v>79.36</v>
       </c>
       <c r="D7" s="16">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="3"/>
@@ -9490,10 +9492,10 @@
       </c>
       <c r="C8" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>73.599999999999994</v>
+        <v>75.2</v>
       </c>
       <c r="D8" s="16">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="3"/>
@@ -9518,10 +9520,10 @@
       </c>
       <c r="C9" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>69.12</v>
+        <v>71.039999999999992</v>
       </c>
       <c r="D9" s="16">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="3"/>
@@ -9546,10 +9548,10 @@
       </c>
       <c r="C10" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>64.64</v>
+        <v>66.88</v>
       </c>
       <c r="D10" s="16">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="3"/>
@@ -9574,10 +9576,10 @@
       </c>
       <c r="C11" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>60.16</v>
+        <v>62.72</v>
       </c>
       <c r="D11" s="16">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="3"/>
@@ -9602,10 +9604,10 @@
       </c>
       <c r="C12" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>55.679999999999993</v>
+        <v>58.56</v>
       </c>
       <c r="D12" s="16">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="3"/>
@@ -9630,10 +9632,10 @@
       </c>
       <c r="C13" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>51.199999999999996</v>
+        <v>54.4</v>
       </c>
       <c r="D13" s="16">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="3"/>
@@ -9658,10 +9660,10 @@
       </c>
       <c r="C14" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>46.72</v>
+        <v>50.239999999999995</v>
       </c>
       <c r="D14" s="16">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -9686,10 +9688,10 @@
       </c>
       <c r="C15" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>42.239999999999995</v>
+        <v>46.08</v>
       </c>
       <c r="D15" s="16">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -9714,10 +9716,10 @@
       </c>
       <c r="C16" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>37.759999999999991</v>
+        <v>41.92</v>
       </c>
       <c r="D16" s="16">
-        <v>59</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9730,10 +9732,10 @@
       </c>
       <c r="C17" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>33.279999999999994</v>
+        <v>37.76</v>
       </c>
       <c r="D17" s="16">
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9746,10 +9748,10 @@
       </c>
       <c r="C18" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>28.799999999999997</v>
+        <v>33.599999999999994</v>
       </c>
       <c r="D18" s="16">
-        <v>59</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9762,10 +9764,10 @@
       </c>
       <c r="C19" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>24.319999999999993</v>
+        <v>29.439999999999998</v>
       </c>
       <c r="D19" s="16">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9778,10 +9780,10 @@
       </c>
       <c r="C20" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>19.839999999999989</v>
+        <v>25.28</v>
       </c>
       <c r="D20" s="16">
-        <v>59</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9794,10 +9796,10 @@
       </c>
       <c r="C21" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>15.359999999999985</v>
+        <v>21.120000000000005</v>
       </c>
       <c r="D21" s="16">
-        <v>59</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9810,10 +9812,10 @@
       </c>
       <c r="C22" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>10.879999999999995</v>
+        <v>16.959999999999994</v>
       </c>
       <c r="D22" s="16">
-        <v>59</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9826,10 +9828,10 @@
       </c>
       <c r="C23" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>6.3999999999999915</v>
+        <v>12.799999999999997</v>
       </c>
       <c r="D23" s="16">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9842,10 +9844,10 @@
       </c>
       <c r="C24" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>1.9199999999999875</v>
+        <v>8.64</v>
       </c>
       <c r="D24" s="16">
-        <v>59</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -9858,10 +9860,10 @@
       </c>
       <c r="C25" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>-2.5600000000000023</v>
+        <v>4.4799999999999898</v>
       </c>
       <c r="D25" s="16">
-        <v>59</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>